<commit_message>
Ajout modeles et fonctionnement pieces d'armure
</commit_message>
<xml_diff>
--- a/ConceptionDocument/Assets_List.xlsx
+++ b/ConceptionDocument/Assets_List.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="PawnModels" sheetId="1" r:id="rId1"/>
-    <sheet name="Platforms" sheetId="3" r:id="rId2"/>
-    <sheet name="Environment" sheetId="2" r:id="rId3"/>
+    <sheet name="Environment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -399,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,18 +485,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>